<commit_message>
Retos sesión 6 postwork sesión 5
</commit_message>
<xml_diff>
--- a/Datasets/Postwork/articles-388408_recurso_1.xlsx
+++ b/Datasets/Postwork/articles-388408_recurso_1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A959643-20AB-4223-BC81-4E8764D85104}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A959643-20AB-4223-BC81-4E8764D85104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -497,13 +497,13 @@
     <xf numFmtId="4" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -847,53 +847,53 @@
   <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.77734375" customWidth="1"/>
-    <col min="2" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="5" width="28.77734375" customWidth="1"/>
-    <col min="6" max="6" width="95.21875" customWidth="1"/>
+    <col min="1" max="1" width="38.7109375" customWidth="1"/>
+    <col min="2" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" customWidth="1"/>
+    <col min="6" max="6" width="95.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="63.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="63.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -910,7 +910,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>1984</v>
       </c>
@@ -925,7 +925,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>1985</v>
       </c>
@@ -942,7 +942,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>1986</v>
       </c>
@@ -959,7 +959,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>1987</v>
       </c>
@@ -976,7 +976,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>1988</v>
       </c>
@@ -993,7 +993,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>1989</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>1990</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>1991</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>1992</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>1993</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>1994</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>1995</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>1996</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>1997</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>1998</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>1999</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>2000</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>2001</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>2002</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>2003</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>2004</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>2005</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>2006</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>2007</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>2008</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>2009</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>2010</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>2011</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>2012</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>2013</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>2014</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>2015</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>2016</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
         <v>2017</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>2018</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10">
         <v>2019</v>
       </c>
@@ -1520,7 +1520,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>2020</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10">
         <v>2021</v>
       </c>
@@ -1554,103 +1554,108 @@
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="17" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="17"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="17" t="s">
+      <c r="B46" s="15"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="17"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="17" t="s">
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B48" s="17"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="17" t="s">
+      <c r="B48" s="15"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="17"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="17" t="s">
+      <c r="B49" s="15"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B50" s="17"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="17" t="s">
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="B51" s="17"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="17" t="s">
+      <c r="B51" s="15"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="17"/>
-      <c r="C52" s="17"/>
-      <c r="D52" s="17"/>
-      <c r="E52" s="17"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="17" t="s">
+      <c r="B52" s="15"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B53" s="17"/>
-      <c r="C53" s="17"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="17"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="17" t="s">
+      <c r="B53" s="15"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B54" s="17"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="17"/>
-      <c r="E54" s="17"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="17" t="s">
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B55" s="17"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A48:E48"/>
     <mergeCell ref="A54:E54"/>
     <mergeCell ref="A55:E55"/>
     <mergeCell ref="A49:E49"/>
@@ -1658,11 +1663,6 @@
     <mergeCell ref="A51:E51"/>
     <mergeCell ref="A52:E52"/>
     <mergeCell ref="A53:E53"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="A48:E48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A47" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>